<commit_message>
Update ArcStructure in ARCTokenizationTests
</commit_message>
<xml_diff>
--- a/tests/ARCTokenization.Tests/Fixtures/arcStructure/assays/measurement1/isa.assay.xlsx
+++ b/tests/ARCTokenization.Tests/Fixtures/arcStructure/assays/measurement1/isa.assay.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lux-c\source\repos\fslaborg\ARCTokenization\tests\ARCTokenization.Tests\Fixtures\testPaths\arcStructure\assays\measurement1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\ARCTokenization\tests\ARCTokenization.Tests\Fixtures\correct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD4AFD2-D295-4044-8E50-3618A12D9902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E668141-CA13-42CA-A99A-B60D96B59874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="isa_assay" sheetId="2" r:id="rId1"/>
+    <sheet name="Cell Lysis" sheetId="1" r:id="rId1"/>
+    <sheet name="Protein Extraction" sheetId="3" r:id="rId2"/>
+    <sheet name="Protein Measurement" sheetId="4" r:id="rId3"/>
+    <sheet name="Computational Proteome Analysis" sheetId="5" r:id="rId4"/>
+    <sheet name="isa_assay" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,74 +37,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
-  <si>
-    <t>Measurement Type</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Measurement Type Term Accession Number</t>
-  </si>
-  <si>
-    <t>Measurement Type Term Source REF</t>
-  </si>
-  <si>
-    <t>Technology Type</t>
-  </si>
-  <si>
-    <t>Technology Type Term Accession Number</t>
-  </si>
-  <si>
-    <t>Technology Type Term Source REF</t>
-  </si>
-  <si>
-    <t>Technology Platform</t>
-  </si>
-  <si>
-    <t>File Name</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="96">
+  <si>
+    <t>measurement1\isa.assay.xlsx</t>
   </si>
   <si>
     <t>ASSAY PERFORMERS</t>
   </si>
   <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Mid Initials</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Fax</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Affiliation</t>
-  </si>
-  <si>
-    <t>Roles</t>
-  </si>
-  <si>
-    <t>Roles Term Accession Number</t>
-  </si>
-  <si>
-    <t>Roles Term Source REF</t>
-  </si>
-  <si>
-    <t>Comment[&lt;Worksheet&gt;]</t>
-  </si>
-  <si>
     <t>Maus</t>
   </si>
   <si>
@@ -122,17 +66,275 @@
     <t>scoro</t>
   </si>
   <si>
+    <t>Source Name</t>
+  </si>
+  <si>
+    <t>Sample Name</t>
+  </si>
+  <si>
+    <t>Cultivation flask</t>
+  </si>
+  <si>
+    <t>Parameter [cell lysis]</t>
+  </si>
+  <si>
+    <t>Term Source REF (OBI:0302894)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (OBI:0302894)</t>
+  </si>
+  <si>
+    <t>sample eppi 1</t>
+  </si>
+  <si>
+    <t>sample eppi 2</t>
+  </si>
+  <si>
+    <t>sample eppi 3</t>
+  </si>
+  <si>
+    <t>sample eppi 4</t>
+  </si>
+  <si>
+    <t>sample eppi 5</t>
+  </si>
+  <si>
+    <t>sample eppi 6</t>
+  </si>
+  <si>
+    <t>sample eppi 7</t>
+  </si>
+  <si>
+    <t>user-specific</t>
+  </si>
+  <si>
+    <t>Sonication</t>
+  </si>
+  <si>
+    <t>NCIT</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C81871</t>
+  </si>
+  <si>
+    <t>Component [sonicator]</t>
+  </si>
+  <si>
+    <t>Term Source REF (OBI:0400114)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (OBI:0400114)</t>
+  </si>
+  <si>
+    <t>Fisherbrand™ Model 705 Sonic Dismembrator</t>
+  </si>
+  <si>
+    <t>Parameter [centrifugation]</t>
+  </si>
+  <si>
+    <t>Term Source REF (OBI:0302886)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (OBI:0302886)</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>g unit</t>
+  </si>
+  <si>
+    <t>Component [centrifuge]</t>
+  </si>
+  <si>
+    <t>Term Source REF (OBI:0400106)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (OBI:0400106)</t>
+  </si>
+  <si>
+    <t>Eppendorf™ Centrifuge 5420</t>
+  </si>
+  <si>
+    <t>Protocol REF</t>
+  </si>
+  <si>
+    <t>extractionProtocol.txt</t>
+  </si>
+  <si>
+    <t>sample eppi extracted 1</t>
+  </si>
+  <si>
+    <t>sample eppi extracted 2</t>
+  </si>
+  <si>
+    <t>sample eppi extracted 3</t>
+  </si>
+  <si>
+    <t>sample eppi extracted 4</t>
+  </si>
+  <si>
+    <t>sample eppi extracted 5</t>
+  </si>
+  <si>
+    <t>sample eppi extracted 6</t>
+  </si>
+  <si>
+    <t>sample eppi extracted 7</t>
+  </si>
+  <si>
+    <t>Derived Data File</t>
+  </si>
+  <si>
+    <t>Raw Data File</t>
+  </si>
+  <si>
+    <t>sample1.raw</t>
+  </si>
+  <si>
+    <t>sample2.raw</t>
+  </si>
+  <si>
+    <t>sample3.raw</t>
+  </si>
+  <si>
+    <t>sample4.raw</t>
+  </si>
+  <si>
+    <t>sample5.raw</t>
+  </si>
+  <si>
+    <t>sample6.raw</t>
+  </si>
+  <si>
+    <t>sample7.raw</t>
+  </si>
+  <si>
+    <t>Term Source REF (MS:1001045)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (MS:1001045)</t>
+  </si>
+  <si>
+    <t>Trypsin</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1001251</t>
+  </si>
+  <si>
+    <t>Term Source REF (MS:1000031)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (MS:1000031)</t>
+  </si>
+  <si>
+    <t>TripleTOF 5600+</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/MS_1002584</t>
+  </si>
+  <si>
+    <t>Component [cleavage agent name]</t>
+  </si>
+  <si>
+    <t>Component [instrument model]</t>
+  </si>
+  <si>
+    <t>Parameter [software]</t>
+  </si>
+  <si>
+    <t>Term Source REF (MS:1000531)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (MS:1000531)</t>
+  </si>
+  <si>
+    <t>ProteomIqon</t>
+  </si>
+  <si>
+    <t>proteomics_results.csv</t>
+  </si>
+  <si>
+    <t>Katz</t>
+  </si>
+  <si>
+    <t>Marius</t>
+  </si>
+  <si>
+    <t>G.</t>
+  </si>
+  <si>
+    <t>Assay Measurement Type</t>
+  </si>
+  <si>
+    <t>Assay Measurement Type Term Accession Number</t>
+  </si>
+  <si>
+    <t>Assay Measurement Type Term Source REF</t>
+  </si>
+  <si>
+    <t>Assay Technology Type</t>
+  </si>
+  <si>
+    <t>Assay Technology Type Term Accession Number</t>
+  </si>
+  <si>
+    <t>Assay Technology Type Term Source REF</t>
+  </si>
+  <si>
+    <t>Assay Technology Platform</t>
+  </si>
+  <si>
+    <t>Assay File Name</t>
+  </si>
+  <si>
+    <t>Assay Performer Last Name</t>
+  </si>
+  <si>
+    <t>Assay Performer First Name</t>
+  </si>
+  <si>
+    <t>Assay Performer Mid Initials</t>
+  </si>
+  <si>
+    <t>Assay Performer Email</t>
+  </si>
+  <si>
+    <t>Assay Performer Phone</t>
+  </si>
+  <si>
+    <t>Assay Performer Fax</t>
+  </si>
+  <si>
+    <t>Assay Performer Address</t>
+  </si>
+  <si>
+    <t>Assay Performer Affiliation</t>
+  </si>
+  <si>
+    <t>Assay Performer Roles</t>
+  </si>
+  <si>
+    <t>Assay Performer Roles Term Accession Number</t>
+  </si>
+  <si>
+    <t>Assay Performer Roles Term Source REF</t>
+  </si>
+  <si>
     <t>ASSAY</t>
-  </si>
-  <si>
-    <t>assays\measurement1\isa.assay.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00\ &quot;g unit&quot;"/>
+  </numFmts>
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +473,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -618,56 +826,119 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Link" xfId="42" builtinId="8"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="20">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -680,8 +951,75 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B52DBDFF-24DA-4BE8-A52A-F407FA0E4B4D}" name="annotationTableStupidQuail41" displayName="annotationTableStupidQuail41" ref="A1:O8" totalsRowShown="0">
+  <autoFilter ref="A1:O8" xr:uid="{B52DBDFF-24DA-4BE8-A52A-F407FA0E4B4D}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{B4197EBB-5C29-48B4-90CD-F088D88B65B5}" name="Source Name"/>
+    <tableColumn id="3" xr3:uid="{EDA29537-390E-4E97-B3E3-3215826FCF7A}" name="Parameter [cell lysis]" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{49DDB123-105B-4A3E-B4F9-32C4BF8EF930}" name="Term Source REF (OBI:0302894)" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{E193D54A-34FA-49EE-A537-096D020E8A01}" name="Term Accession Number (OBI:0302894)" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{1B84D55D-096C-4F04-AA09-4D38A24384AB}" name="Component [sonicator]" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{9396F106-FB08-4259-A27A-9D91BBBFF5C1}" name="Term Source REF (OBI:0400114)" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{6483C350-F7C5-4740-8A4A-F79450CE13DE}" name="Term Accession Number (OBI:0400114)" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{21DADCF8-A145-435A-BC82-DCB11449D43B}" name="Parameter [centrifugation]" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{EB509DE1-F9E5-4184-AFC2-F3085834D809}" name="Unit" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{94F72135-931B-419A-A66E-48B1C79588E5}" name="Term Source REF (OBI:0302886)" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{DAC32DA4-F07B-40AF-BE70-C1792062AB41}" name="Term Accession Number (OBI:0302886)" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{3C99F4F2-96D1-420F-A889-99946E31F7F7}" name="Component [centrifuge]" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{2516674C-3D96-42FF-A079-5A99EBFACE29}" name="Term Source REF (OBI:0400106)" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{EDF4E12B-7169-44D1-BB36-537B6AF363C5}" name="Term Accession Number (OBI:0400106)" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{DE4D389F-1A14-4220-ADFD-518EC3ACEF11}" name="Sample Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A63CC62-0D13-40AE-BA14-DC568C11E28E}" name="annotationTableWittyFox29" displayName="annotationTableWittyFox29" ref="A1:C8" totalsRowShown="0">
+  <autoFilter ref="A1:C8" xr:uid="{4A63CC62-0D13-40AE-BA14-DC568C11E28E}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{2EC0724E-B90C-4D11-9DDA-5D7A7CF4FE4B}" name="Source Name"/>
+    <tableColumn id="3" xr3:uid="{1E3EC630-9159-4CC1-9D82-8F84409216A0}" name="Protocol REF"/>
+    <tableColumn id="2" xr3:uid="{E4ABA81E-FD30-49BF-BC32-78010366A942}" name="Sample Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{A8F00DCA-82D9-495E-85A8-EBC9EEE0CB19}" name="annotationTableWeakSnake44" displayName="annotationTableWeakSnake44" ref="A1:H8" totalsRowShown="0">
+  <autoFilter ref="A1:H8" xr:uid="{A8F00DCA-82D9-495E-85A8-EBC9EEE0CB19}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{B8D6909B-B26C-4766-B0A1-2B354A37F270}" name="Source Name"/>
+    <tableColumn id="6" xr3:uid="{90131BA9-CBB2-4C80-A900-1A8C6407588F}" name="Component [cleavage agent name]"/>
+    <tableColumn id="7" xr3:uid="{DFBB533C-F7ED-4A36-8C59-F947F2252499}" name="Term Source REF (MS:1001045)" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{82408F10-2085-46D5-BAF0-C4E7C4B53AF2}" name="Term Accession Number (MS:1001045)" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{0A562C5D-7742-4D6C-BC10-C03AB2BC1BA7}" name="Component [instrument model]" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{63F81720-D120-4D4F-8536-894E68C839A9}" name="Term Source REF (MS:1000031)" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{31DE825E-55C0-41C8-A948-6445D9817E03}" name="Term Accession Number (MS:1000031)" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{400C3C8E-6524-46F1-B712-F67011267FF9}" name="Raw Data File"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{78B8F38D-9BAC-4B0E-9330-763AAFE8CA12}" name="annotationTablePurplePanther50" displayName="annotationTablePurplePanther50" ref="A1:E8" totalsRowShown="0">
+  <autoFilter ref="A1:E8" xr:uid="{78B8F38D-9BAC-4B0E-9330-763AAFE8CA12}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A0AC472A-21A4-4E95-8FD5-0B20DE388BEE}" name="Source Name"/>
+    <tableColumn id="3" xr3:uid="{C2033594-D549-4BF3-AFC7-F7E458EFF1C1}" name="Parameter [software]"/>
+    <tableColumn id="4" xr3:uid="{D0ED9002-6C32-403F-A17C-33D0B3BC25A8}" name="Term Source REF (MS:1000531)" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{69476E4A-15DA-41A7-B39A-4D20058CFB98}" name="Term Accession Number (MS:1000531)" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{569AE1B2-54A1-474C-9318-1F9AD38E9F9A}" name="Derived Data File"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -994,187 +1332,1066 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="3">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="3">
+        <v>10</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="3">
+        <v>10</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="3">
+        <v>10</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="3">
+        <v>10</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="3">
+        <v>10</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED622AF-C6D3-4178-A922-80BD7864C242}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3801D409-B8B0-4855-BA5A-150CE30B4552}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="37.5703125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645D591A-BDF3-41CD-9608-14D46BCB1811}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" t="s">
         <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expand metadata tokenisation (#57)
* Update Metadata references

* Update ReferenceObjects.fs

Update ReferenceObjects to utilise Assay Person instead of the old Assay Performer

* Update testing

* Update FileSystemTokenization Test

* Adapt ARCMock to allow for empty fields to be deleted

- Change ARCMock functions
- Fix Tests using ARCMock
</commit_message>
<xml_diff>
--- a/tests/ARCTokenization.Tests/Fixtures/arcStructure/assays/measurement1/isa.assay.xlsx
+++ b/tests/ARCTokenization.Tests/Fixtures/arcStructure/assays/measurement1/isa.assay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\ARCTokenization\tests\ARCTokenization.Tests\Fixtures\correct\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chris\forARC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E668141-CA13-42CA-A99A-B60D96B59874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8117AD4-B30F-4D54-8CB7-39EB53CC4BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="5625" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cell Lysis" sheetId="1" r:id="rId1"/>
@@ -291,40 +291,40 @@
     <t>Assay File Name</t>
   </si>
   <si>
-    <t>Assay Performer Last Name</t>
-  </si>
-  <si>
-    <t>Assay Performer First Name</t>
-  </si>
-  <si>
-    <t>Assay Performer Mid Initials</t>
-  </si>
-  <si>
-    <t>Assay Performer Email</t>
-  </si>
-  <si>
-    <t>Assay Performer Phone</t>
-  </si>
-  <si>
-    <t>Assay Performer Fax</t>
-  </si>
-  <si>
-    <t>Assay Performer Address</t>
-  </si>
-  <si>
-    <t>Assay Performer Affiliation</t>
-  </si>
-  <si>
-    <t>Assay Performer Roles</t>
-  </si>
-  <si>
-    <t>Assay Performer Roles Term Accession Number</t>
-  </si>
-  <si>
-    <t>Assay Performer Roles Term Source REF</t>
-  </si>
-  <si>
     <t>ASSAY</t>
+  </si>
+  <si>
+    <t>Assay Person Last Name</t>
+  </si>
+  <si>
+    <t>Assay Person First Name</t>
+  </si>
+  <si>
+    <t>Assay Person Mid Initials</t>
+  </si>
+  <si>
+    <t>Assay Person Email</t>
+  </si>
+  <si>
+    <t>Assay Person Phone</t>
+  </si>
+  <si>
+    <t>Assay Person Fax</t>
+  </si>
+  <si>
+    <t>Assay Person Address</t>
+  </si>
+  <si>
+    <t>Assay Person Affiliation</t>
+  </si>
+  <si>
+    <t>Assay Person Roles</t>
+  </si>
+  <si>
+    <t>Assay Person Roles Term Accession Number</t>
+  </si>
+  <si>
+    <t>Assay Person Roles Term Source REF</t>
   </si>
 </sst>
 </file>
@@ -833,49 +833,49 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Link" xfId="42" builtinId="8"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="20">
     <dxf>
@@ -1019,9 +1019,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1059,7 +1059,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1165,7 +1165,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1307,7 +1307,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1337,7 +1337,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
@@ -1747,7 +1747,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
@@ -1857,7 +1857,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
@@ -2091,7 +2091,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
@@ -2248,9 +2248,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.85546875" bestFit="1" customWidth="1"/>
@@ -2258,7 +2260,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2311,7 +2313,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -2322,7 +2324,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -2333,7 +2335,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C13" t="s">
         <v>75</v>
@@ -2341,7 +2343,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>4</v>
@@ -2349,22 +2351,22 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -2372,7 +2374,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -2380,7 +2382,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>7</v>
@@ -2388,7 +2390,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>

</xml_diff>